<commit_message>
Refined files and redone analysis
</commit_message>
<xml_diff>
--- a/SourceDataTables/Fig2b.xlsx
+++ b/SourceDataTables/Fig2b.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Thalamic_ROI</t>
   </si>
@@ -144,7 +144,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -154,34 +154,14 @@
     </border>
     <border/>
     <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -199,15 +179,15 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2">
@@ -215,7 +195,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3">
@@ -223,7 +203,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4">
@@ -231,7 +211,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5">
@@ -239,7 +219,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6">
@@ -247,7 +227,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B7">
@@ -255,7 +235,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B8">
@@ -263,7 +243,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B9">
@@ -271,7 +251,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B10">
@@ -279,7 +259,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B11">
@@ -287,7 +267,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B12">
@@ -295,7 +275,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B13">
@@ -303,7 +283,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B14">
@@ -311,7 +291,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B15">
@@ -319,7 +299,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B16">
@@ -327,7 +307,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B17">
@@ -335,7 +315,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B18">
@@ -343,7 +323,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B19">
@@ -351,7 +331,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B20">
@@ -359,7 +339,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B21">
@@ -367,7 +347,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B22">
@@ -375,7 +355,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B23">
@@ -383,7 +363,7 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B24">
@@ -391,7 +371,7 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="11" t="s">
+      <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B25">
@@ -399,7 +379,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B26">
@@ -407,7 +387,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B27">
@@ -415,7 +395,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="11" t="s">
+      <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B28">
@@ -423,7 +403,7 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="11" t="s">
+      <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B29">
@@ -431,7 +411,7 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="11" t="s">
+      <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B30">
@@ -439,7 +419,7 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B31">
@@ -447,7 +427,7 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="11" t="s">
+      <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B32">
@@ -455,7 +435,7 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="11" t="s">
+      <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B33">
@@ -463,7 +443,7 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="11" t="s">
+      <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B34">
@@ -471,7 +451,7 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="11" t="s">
+      <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B35">
@@ -479,7 +459,7 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="11" t="s">
+      <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B36">

</xml_diff>